<commit_message>
Add dummy data to excel files
</commit_message>
<xml_diff>
--- a/fraternity_submission_template.xlsx
+++ b/fraternity_submission_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackditto/Hobby/Programming/Lodge-List-Checker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1BBBE36-E6A7-E04C-BD66-AAB4F68128E7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF208B5-7172-D347-8EA9-F075567C8ECC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8220" yWindow="600" windowWidth="20640" windowHeight="15880" xr2:uid="{E80BB752-6B25-604E-B5DC-03B520D2C417}"/>
+    <workbookView xWindow="13060" yWindow="500" windowWidth="20640" windowHeight="15880" xr2:uid="{E80BB752-6B25-604E-B5DC-03B520D2C417}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>First Name</t>
   </si>
@@ -40,6 +40,36 @@
   </si>
   <si>
     <t>Student ID</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scott </t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Patterson</t>
+  </si>
+  <si>
+    <t>Ditto</t>
+  </si>
+  <si>
+    <t>0000001</t>
+  </si>
+  <si>
+    <t>0000003</t>
+  </si>
+  <si>
+    <t>0000004</t>
   </si>
 </sst>
 </file>
@@ -75,8 +105,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5BC8E52-96E3-AD40-B377-BE6C803E5779}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -410,6 +441,47 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>